<commit_message>
1/19/2020: Add Pre-IX RATFreqPrio selection 01,02,03,04
</commit_message>
<xml_diff>
--- a/references/presrt_template.xlsx
+++ b/references/presrt_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\srtwp\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B249A846-E5D0-4C6D-B34B-895FDE7CF423}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C192DF-60A6-45E7-BFA6-9C6B8FEA2F17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="36499" windowHeight="11135" xr2:uid="{0E83E68F-0426-4499-8C0C-19C675E5B902}"/>
+    <workbookView xWindow="33395" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{0E83E68F-0426-4499-8C0C-19C675E5B902}"/>
   </bookViews>
   <sheets>
     <sheet name="CellData" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t>noOfTxAntennas</t>
-  </si>
-  <si>
     <t>earfcnDl</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>Post.eNBId</t>
+  </si>
+  <si>
+    <t>noOfRxAntennas</t>
   </si>
 </sst>
 </file>
@@ -470,81 +470,81 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="A1:Q1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
     <col min="15" max="16" width="21" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>